<commit_message>
smenena cena na presto salad shootera
</commit_message>
<xml_diff>
--- a/GlobalTrusted.xlsx
+++ b/GlobalTrusted.xlsx
@@ -2931,8 +2931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4449,49 +4449,48 @@
         <v>55</v>
       </c>
       <c r="E24" s="30">
-        <v>27.99</v>
+        <v>29.99</v>
       </c>
       <c r="F24" s="31">
         <f t="shared" si="6"/>
-        <v>2.2391999999999999</v>
+        <v>2.3992</v>
       </c>
       <c r="G24" s="20">
         <v>0</v>
       </c>
       <c r="H24" s="28">
         <f t="shared" si="0"/>
-        <v>5.1389640000000005</v>
+        <v>5.5061639999999992</v>
       </c>
       <c r="I24" s="34">
         <f t="shared" si="1"/>
-        <v>35.368164</v>
+        <v>37.895363999999994</v>
       </c>
       <c r="J24" s="22">
-        <f t="shared" si="10"/>
-        <v>37.932048000000002</v>
+        <v>42.95</v>
       </c>
       <c r="K24" s="28">
         <f t="shared" si="7"/>
-        <v>6.4936799999999995</v>
+        <v>6.9576799999999999</v>
       </c>
       <c r="L24" s="29">
         <f t="shared" si="2"/>
-        <v>30.229199999999999</v>
+        <v>32.389199999999995</v>
       </c>
       <c r="M24" s="37">
         <f t="shared" si="3"/>
-        <v>37.932048000000002</v>
+        <v>40.642448000000002</v>
       </c>
       <c r="N24" s="37">
         <f t="shared" si="8"/>
-        <v>3.4483680000000021</v>
+        <v>6.0023200000000045</v>
       </c>
       <c r="O24" s="36">
         <v>0</v>
       </c>
       <c r="P24" s="32">
         <f t="shared" si="4"/>
-        <v>3.4483680000000021</v>
+        <v>6.0023200000000045</v>
       </c>
       <c r="Q24" s="33">
         <f t="shared" si="11"/>
@@ -4499,7 +4498,7 @@
       </c>
       <c r="R24" s="38">
         <f t="shared" si="9"/>
-        <v>0.10000000000000006</v>
+        <v>0.16245458442857588</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>